<commit_message>
fix:Stepped revision of excel file
Signed-off-by: Fredrik Nordlander <fredrik.nordlander@digg.se>
</commit_message>
<xml_diff>
--- a/document/Avstaemning_REST_API_profil_v_1_2_0_0.xlsx
+++ b/document/Avstaemning_REST_API_profil_v_1_2_0_0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FV2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FV2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" tabRatio="692"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="13800" tabRatio="692"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -3513,53 +3513,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mellan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Exponering av interna systemidentifierare </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BÖR INTE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (exempelvis ett databas-ID) med konsumenter.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Felmeddelanden </t>
     </r>
     <r>
@@ -6222,6 +6175,53 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">  anges i URL enligt formatet v[x] där 'v' avser förkortning för version och x avser ett och bara ett nummer (0-n) för major-version</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mellan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Exponering av interna systemidentifierare </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BÖR INTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (exempelvis ett databas-ID) exponeras till konsumenter.</t>
     </r>
   </si>
 </sst>
@@ -6928,6 +6928,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6954,9 +6957,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -7373,74 +7373,74 @@
   <dimension ref="A1:AW48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+      <selection activeCell="A2" sqref="A2:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="22" customWidth="1"/>
-    <col min="2" max="13" width="10.7265625" style="16" customWidth="1"/>
-    <col min="14" max="49" width="8.7265625" style="16"/>
+    <col min="1" max="1" width="10.7109375" style="22" customWidth="1"/>
+    <col min="2" max="13" width="10.7109375" style="16" customWidth="1"/>
+    <col min="14" max="49" width="8.7109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:24" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-    </row>
-    <row r="2" spans="1:24" ht="155.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="77" t="s">
-        <v>371</v>
-      </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78" t="s">
-        <v>330</v>
-      </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+    </row>
+    <row r="2" spans="1:24" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="81"/>
       <c r="X2" s="29"/>
     </row>
-    <row r="3" spans="1:24" s="37" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="37" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -7448,12 +7448,12 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:24" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>134</v>
       </c>
@@ -7467,10 +7467,10 @@
         <v>133</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <f>COUNTIF('Kravlista REST API profil'!E2:E190,"-")</f>
         <v>151</v>
@@ -7495,7 +7495,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <f>(A6/SUM(A6:E6))</f>
         <v>1</v>
@@ -7520,12 +7520,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="str">
         <f>('Kravlista REST API profil'!$A2)</f>
         <v>Dokumentation</v>
@@ -7535,7 +7535,7 @@
         <v>Datum- och tidsformat</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -7577,7 +7577,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E2:E26,"-")</f>
         <v>23</v>
@@ -7625,7 +7625,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <f>(A12/SUM(A12:E12))</f>
         <v>1</v>
@@ -7673,7 +7673,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="str">
         <f>('Kravlista REST API profil'!$A33)</f>
         <v>Resurser</v>
@@ -7683,7 +7683,7 @@
         <v>URL format och namngivning</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -7725,7 +7725,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E33:E40,"-")</f>
         <v>6</v>
@@ -7773,7 +7773,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <f>(A17/SUM(A17:E17))</f>
         <v>1</v>
@@ -7821,7 +7821,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="str">
         <f>('Kravlista REST API profil'!$A52)</f>
         <v>Mognad</v>
@@ -7831,7 +7831,7 @@
         <v>Säkerhet</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -7873,7 +7873,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E52:E54,"-")</f>
         <v>3</v>
@@ -7921,7 +7921,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26">
         <f>(A22/SUM(A22:E22))</f>
         <v>1</v>
@@ -7969,7 +7969,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="str">
         <f>('Kravlista REST API profil'!$A97)</f>
         <v>API Message</v>
@@ -7979,7 +7979,7 @@
         <v>API Request</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -8021,7 +8021,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E97:E104,"-")</f>
         <v>6</v>
@@ -8069,7 +8069,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26">
         <f>(A27/SUM(A27:E27))</f>
         <v>1</v>
@@ -8117,7 +8117,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="str">
         <f>('Kravlista REST API profil'!$A112)</f>
         <v>API Response</v>
@@ -8127,7 +8127,7 @@
         <v>Felhantering</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -8169,7 +8169,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E112:E115,"-")</f>
         <v>3</v>
@@ -8217,7 +8217,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26">
         <f>(A32/SUM(A32:E32))</f>
         <v>1</v>
@@ -8265,7 +8265,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="str">
         <f>('Kravlista REST API profil'!$A118)</f>
         <v>Versionshantering</v>
@@ -8275,7 +8275,7 @@
         <v>Webhooks</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -8317,7 +8317,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E118:E142,"-")</f>
         <v>19</v>
@@ -8365,7 +8365,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26">
         <f>(A37/SUM(A37:E37))</f>
         <v>1</v>
@@ -8413,7 +8413,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="str">
         <f>('Kravlista REST API profil'!$A149)</f>
         <v>Hypermedia</v>
@@ -8423,7 +8423,7 @@
         <v>Filtrering, namnsättning och sökparametrar</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -8465,7 +8465,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E149:E173,"-")</f>
         <v>19</v>
@@ -8513,7 +8513,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26">
         <f>(A42/SUM(A42:E42))</f>
         <v>1</v>
@@ -8561,13 +8561,13 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="42" t="str">
         <f>('Kravlista REST API profil'!$A190)</f>
         <v>Cachning</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="str">
         <f>$A$5</f>
         <v>-</v>
@@ -8589,7 +8589,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <f>COUNTIF('Kravlista REST API profil'!E190:E190,"-")</f>
         <v>1</v>
@@ -8619,7 +8619,7 @@
       <c r="K47" s="40"/>
       <c r="L47" s="40"/>
     </row>
-    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26">
         <f>(A47/SUM(A47:E47))</f>
         <v>1</v>
@@ -8666,23 +8666,23 @@
   <dimension ref="A1:BJ418"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="92.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="34" customWidth="1"/>
-    <col min="6" max="6" width="38.54296875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="12"/>
-    <col min="8" max="62" width="8.7265625" style="10"/>
-    <col min="63" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="11.140625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="12"/>
+    <col min="8" max="62" width="8.7109375" style="10"/>
+    <col min="63" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -8758,12 +8758,12 @@
       <c r="BI1" s="10"/>
       <c r="BJ1" s="10"/>
     </row>
-    <row r="2" spans="1:62" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:62" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>43</v>
@@ -8777,10 +8777,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:62" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:62" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
       <c r="B3" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -8794,7 +8794,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60"/>
       <c r="B4" s="38" t="s">
         <v>5</v>
@@ -8805,10 +8805,10 @@
       <c r="F4" s="47"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:62" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:62" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>137</v>
@@ -8822,10 +8822,10 @@
       <c r="F5" s="4"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:62" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:62" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>44</v>
@@ -8839,10 +8839,10 @@
       <c r="F6" s="4"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>45</v>
@@ -8856,10 +8856,10 @@
       <c r="F7" s="4"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>46</v>
@@ -8873,10 +8873,10 @@
       <c r="F8" s="4"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>47</v>
@@ -8890,10 +8890,10 @@
       <c r="F9" s="4"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>48</v>
@@ -8907,10 +8907,10 @@
       <c r="F10" s="4"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>49</v>
@@ -8924,10 +8924,10 @@
       <c r="F11" s="4"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>138</v>
@@ -8941,10 +8941,10 @@
       <c r="F12" s="4"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>50</v>
@@ -8958,10 +8958,10 @@
       <c r="F13" s="4"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:62" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:62" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>139</v>
@@ -8975,10 +8975,10 @@
       <c r="F14" s="4"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>51</v>
@@ -8992,10 +8992,10 @@
       <c r="F15" s="4"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:62" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:62" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>52</v>
@@ -9009,7 +9009,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="38" t="s">
         <v>6</v>
@@ -9020,10 +9020,10 @@
       <c r="F17" s="47"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>87</v>
@@ -9037,13 +9037,13 @@
       <c r="F18" s="4"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="60"/>
       <c r="B19" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
@@ -9054,10 +9054,10 @@
       <c r="F19" s="4"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="60"/>
       <c r="B20" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>140</v>
@@ -9071,10 +9071,10 @@
       <c r="F20" s="4"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="60"/>
       <c r="B21" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>139</v>
@@ -9088,10 +9088,10 @@
       <c r="F21" s="4"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="60"/>
       <c r="B22" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>51</v>
@@ -9105,10 +9105,10 @@
       <c r="F22" s="4"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="60"/>
       <c r="B23" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>141</v>
@@ -9122,10 +9122,10 @@
       <c r="F23" s="4"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="60"/>
       <c r="B24" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>53</v>
@@ -9139,10 +9139,10 @@
       <c r="F24" s="4"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="60"/>
       <c r="B25" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>54</v>
@@ -9156,10 +9156,10 @@
       <c r="F25" s="4"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="61"/>
       <c r="B26" s="48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="49" t="s">
         <v>142</v>
@@ -9173,12 +9173,12 @@
       <c r="F26" s="49"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A27" s="59" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C27" s="44" t="s">
         <v>85</v>
@@ -9192,7 +9192,7 @@
       <c r="F27" s="43"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="64"/>
       <c r="B28" s="39" t="s">
         <v>118</v>
@@ -9203,10 +9203,10 @@
       <c r="F28" s="47"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
       <c r="B29" s="62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>32</v>
@@ -9220,7 +9220,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="64"/>
       <c r="B30" s="39" t="s">
         <v>119</v>
@@ -9231,10 +9231,10 @@
       <c r="F30" s="47"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="64"/>
       <c r="B31" s="62" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>143</v>
@@ -9248,10 +9248,10 @@
       <c r="F31" s="4"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="65"/>
       <c r="B32" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="49" t="s">
         <v>144</v>
@@ -9265,7 +9265,7 @@
       <c r="F32" s="49"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="s">
         <v>8</v>
       </c>
@@ -9278,10 +9278,10 @@
       <c r="F33" s="53"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>88</v>
@@ -9295,10 +9295,10 @@
       <c r="F34" s="4"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>145</v>
@@ -9312,10 +9312,10 @@
       <c r="F35" s="4"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>55</v>
@@ -9329,10 +9329,10 @@
       <c r="F36" s="4"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>56</v>
@@ -9346,13 +9346,13 @@
       <c r="F37" s="4"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" ht="167" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="167.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>20</v>
@@ -9363,7 +9363,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="38" t="s">
         <v>121</v>
@@ -9374,10 +9374,10 @@
       <c r="F39" s="47"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="61"/>
       <c r="B40" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>147</v>
@@ -9391,7 +9391,7 @@
       <c r="F40" s="49"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="s">
         <v>9</v>
       </c>
@@ -9404,10 +9404,10 @@
       <c r="F41" s="53"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="64"/>
       <c r="B42" s="62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>86</v>
@@ -9421,10 +9421,10 @@
       <c r="F42" s="4"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64"/>
       <c r="B43" s="62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>146</v>
@@ -9438,10 +9438,10 @@
       <c r="F43" s="4"/>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="64"/>
       <c r="B44" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>57</v>
@@ -9455,10 +9455,10 @@
       <c r="F44" s="4"/>
       <c r="G44" s="14"/>
     </row>
-    <row r="45" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A45" s="64"/>
       <c r="B45" s="62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>126</v>
@@ -9472,7 +9472,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64"/>
       <c r="B46" s="39" t="s">
         <v>123</v>
@@ -9483,10 +9483,10 @@
       <c r="F46" s="47"/>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
       <c r="B47" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>148</v>
@@ -9500,7 +9500,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="14"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="64"/>
       <c r="B48" s="39" t="s">
         <v>124</v>
@@ -9511,13 +9511,13 @@
       <c r="F48" s="47"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="64"/>
       <c r="B49" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="C49" s="85" t="s">
-        <v>331</v>
+        <v>237</v>
+      </c>
+      <c r="C49" s="76" t="s">
+        <v>330</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>19</v>
@@ -9528,13 +9528,13 @@
       <c r="F49" s="4"/>
       <c r="G49" s="14"/>
     </row>
-    <row r="50" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A50" s="64"/>
       <c r="B50" s="62" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>19</v>
@@ -9545,13 +9545,13 @@
       <c r="F50" s="4"/>
       <c r="G50" s="14"/>
     </row>
-    <row r="51" spans="1:7" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="65"/>
       <c r="B51" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C51" s="49" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D51" s="49" t="s">
         <v>128</v>
@@ -9562,12 +9562,12 @@
       <c r="F51" s="49"/>
       <c r="G51" s="14"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="64" t="s">
         <v>10</v>
       </c>
       <c r="B52" s="66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C52" s="44" t="s">
         <v>58</v>
@@ -9581,10 +9581,10 @@
       <c r="F52" s="44"/>
       <c r="G52" s="14"/>
     </row>
-    <row r="53" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="64"/>
       <c r="B53" s="62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>59</v>
@@ -9598,10 +9598,10 @@
       <c r="F53" s="4"/>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="65"/>
       <c r="B54" s="63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C54" s="49" t="s">
         <v>60</v>
@@ -9615,7 +9615,7 @@
       <c r="F54" s="49"/>
       <c r="G54" s="14"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="64" t="s">
         <v>21</v>
       </c>
@@ -9628,10 +9628,10 @@
       <c r="F55" s="53"/>
       <c r="G55" s="14"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="64"/>
       <c r="B56" s="62" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>61</v>
@@ -9645,10 +9645,10 @@
       <c r="F56" s="4"/>
       <c r="G56" s="14"/>
     </row>
-    <row r="57" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="64"/>
       <c r="B57" s="62" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>149</v>
@@ -9662,10 +9662,10 @@
       <c r="F57" s="4"/>
       <c r="G57" s="14"/>
     </row>
-    <row r="58" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="64"/>
       <c r="B58" s="62" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>150</v>
@@ -9679,10 +9679,10 @@
       <c r="F58" s="4"/>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="64"/>
       <c r="B59" s="62" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>151</v>
@@ -9696,10 +9696,10 @@
       <c r="F59" s="4"/>
       <c r="G59" s="14"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="64"/>
       <c r="B60" s="62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>152</v>
@@ -9713,10 +9713,10 @@
       <c r="F60" s="4"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="64"/>
       <c r="B61" s="62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>153</v>
@@ -9730,7 +9730,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="14"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="64"/>
       <c r="B62" s="39" t="s">
         <v>93</v>
@@ -9741,10 +9741,10 @@
       <c r="F62" s="47"/>
       <c r="G62" s="14"/>
     </row>
-    <row r="63" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="64"/>
       <c r="B63" s="62" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>154</v>
@@ -9758,10 +9758,10 @@
       <c r="F63" s="4"/>
       <c r="G63" s="14"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="64"/>
       <c r="B64" s="62" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>155</v>
@@ -9775,10 +9775,10 @@
       <c r="F64" s="4"/>
       <c r="G64" s="14"/>
     </row>
-    <row r="65" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="64"/>
       <c r="B65" s="62" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>62</v>
@@ -9792,10 +9792,10 @@
       <c r="F65" s="4"/>
       <c r="G65" s="14"/>
     </row>
-    <row r="66" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A66" s="64"/>
       <c r="B66" s="62" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>156</v>
@@ -9809,10 +9809,10 @@
       <c r="F66" s="4"/>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A67" s="64"/>
       <c r="B67" s="62" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>89</v>
@@ -9826,10 +9826,10 @@
       <c r="F67" s="4"/>
       <c r="G67" s="14"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="64"/>
       <c r="B68" s="62" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>157</v>
@@ -9843,10 +9843,10 @@
       <c r="F68" s="4"/>
       <c r="G68" s="14"/>
     </row>
-    <row r="69" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="64"/>
       <c r="B69" s="62" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>158</v>
@@ -9860,10 +9860,10 @@
       <c r="F69" s="4"/>
       <c r="G69" s="14"/>
     </row>
-    <row r="70" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="64"/>
       <c r="B70" s="62" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>63</v>
@@ -9877,10 +9877,10 @@
       <c r="F70" s="4"/>
       <c r="G70" s="14"/>
     </row>
-    <row r="71" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="64"/>
       <c r="B71" s="62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>90</v>
@@ -9894,7 +9894,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="14"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="64"/>
       <c r="B72" s="39" t="s">
         <v>94</v>
@@ -9905,10 +9905,10 @@
       <c r="F72" s="47"/>
       <c r="G72" s="14"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="64"/>
       <c r="B73" s="62" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>159</v>
@@ -9922,7 +9922,7 @@
       <c r="F73" s="4"/>
       <c r="G73" s="14"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="64"/>
       <c r="B74" s="39" t="s">
         <v>95</v>
@@ -9933,10 +9933,10 @@
       <c r="F74" s="47"/>
       <c r="G74" s="14"/>
     </row>
-    <row r="75" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="64"/>
       <c r="B75" s="62" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>64</v>
@@ -9950,10 +9950,10 @@
       <c r="F75" s="4"/>
       <c r="G75" s="14"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="64"/>
       <c r="B76" s="62" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>160</v>
@@ -9967,10 +9967,10 @@
       <c r="F76" s="4"/>
       <c r="G76" s="14"/>
     </row>
-    <row r="77" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="64"/>
       <c r="B77" s="62" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>161</v>
@@ -9984,13 +9984,13 @@
       <c r="F77" s="4"/>
       <c r="G77" s="14"/>
     </row>
-    <row r="78" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="64"/>
       <c r="B78" s="62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>162</v>
+        <v>374</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>127</v>
@@ -10001,13 +10001,13 @@
       <c r="F78" s="4"/>
       <c r="G78" s="14"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="64"/>
       <c r="B79" s="62" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>20</v>
@@ -10018,7 +10018,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="14"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="64"/>
       <c r="B80" s="39" t="s">
         <v>23</v>
@@ -10029,13 +10029,13 @@
       <c r="F80" s="47"/>
       <c r="G80" s="14"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" s="64"/>
       <c r="B81" s="62" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>128</v>
@@ -10046,13 +10046,13 @@
       <c r="F81" s="4"/>
       <c r="G81" s="14"/>
     </row>
-    <row r="82" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="64"/>
       <c r="B82" s="62" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>19</v>
@@ -10063,13 +10063,13 @@
       <c r="F82" s="4"/>
       <c r="G82" s="14"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A83" s="64"/>
       <c r="B83" s="62" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>128</v>
@@ -10080,7 +10080,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="14"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="64"/>
       <c r="B84" s="39" t="s">
         <v>96</v>
@@ -10091,13 +10091,13 @@
       <c r="F84" s="47"/>
       <c r="G84" s="14"/>
     </row>
-    <row r="85" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="64"/>
       <c r="B85" s="62" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>20</v>
@@ -10108,7 +10108,7 @@
       <c r="F85" s="4"/>
       <c r="G85" s="14"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="64"/>
       <c r="B86" s="39" t="s">
         <v>97</v>
@@ -10119,10 +10119,10 @@
       <c r="F86" s="47"/>
       <c r="G86" s="14"/>
     </row>
-    <row r="87" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="64"/>
       <c r="B87" s="62" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>91</v>
@@ -10136,7 +10136,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="14"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="64"/>
       <c r="B88" s="39" t="s">
         <v>98</v>
@@ -10147,13 +10147,13 @@
       <c r="F88" s="47"/>
       <c r="G88" s="14"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="64"/>
       <c r="B89" s="62" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>20</v>
@@ -10164,7 +10164,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="14"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="64"/>
       <c r="B90" s="39" t="s">
         <v>99</v>
@@ -10175,13 +10175,13 @@
       <c r="F90" s="47"/>
       <c r="G90" s="14"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="64"/>
       <c r="B91" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>20</v>
@@ -10192,13 +10192,13 @@
       <c r="F91" s="4"/>
       <c r="G91" s="14"/>
     </row>
-    <row r="92" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A92" s="64"/>
       <c r="B92" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>20</v>
@@ -10209,13 +10209,13 @@
       <c r="F92" s="4"/>
       <c r="G92" s="14"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="64"/>
       <c r="B93" s="62" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>20</v>
@@ -10226,13 +10226,13 @@
       <c r="F93" s="4"/>
       <c r="G93" s="14"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="64"/>
       <c r="B94" s="62" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>20</v>
@@ -10243,13 +10243,13 @@
       <c r="F94" s="4"/>
       <c r="G94" s="14"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="64"/>
       <c r="B95" s="62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>20</v>
@@ -10260,13 +10260,13 @@
       <c r="F95" s="4"/>
       <c r="G95" s="14"/>
     </row>
-    <row r="96" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="65"/>
       <c r="B96" s="63" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C96" s="49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D96" s="49" t="s">
         <v>20</v>
@@ -10277,15 +10277,15 @@
       <c r="F96" s="49"/>
       <c r="G96" s="14"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="64" t="s">
         <v>11</v>
       </c>
       <c r="B97" s="66" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C97" s="44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D97" s="44" t="s">
         <v>20</v>
@@ -10296,7 +10296,7 @@
       <c r="F97" s="44"/>
       <c r="G97" s="14"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="64"/>
       <c r="B98" s="39" t="s">
         <v>100</v>
@@ -10307,10 +10307,10 @@
       <c r="F98" s="47"/>
       <c r="G98" s="14"/>
     </row>
-    <row r="99" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="64"/>
       <c r="B99" s="62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>65</v>
@@ -10324,7 +10324,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="14"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="64"/>
       <c r="B100" s="39" t="s">
         <v>101</v>
@@ -10335,13 +10335,13 @@
       <c r="F100" s="47"/>
       <c r="G100" s="14"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="64"/>
       <c r="B101" s="62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>20</v>
@@ -10352,13 +10352,13 @@
       <c r="F101" s="4"/>
       <c r="G101" s="14"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A102" s="64"/>
       <c r="B102" s="62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>19</v>
@@ -10369,10 +10369,10 @@
       <c r="F102" s="4"/>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="64"/>
       <c r="B103" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>66</v>
@@ -10386,13 +10386,13 @@
       <c r="F103" s="4"/>
       <c r="G103" s="14"/>
     </row>
-    <row r="104" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="65"/>
       <c r="B104" s="63" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D104" s="49" t="s">
         <v>20</v>
@@ -10403,15 +10403,15 @@
       <c r="F104" s="49"/>
       <c r="G104" s="14"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="67" t="s">
         <v>12</v>
       </c>
       <c r="B105" s="66" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C105" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D105" s="44" t="s">
         <v>20</v>
@@ -10422,7 +10422,7 @@
       <c r="F105" s="44"/>
       <c r="G105" s="14"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="64"/>
       <c r="B106" s="39" t="s">
         <v>102</v>
@@ -10433,13 +10433,13 @@
       <c r="F106" s="47"/>
       <c r="G106" s="14"/>
     </row>
-    <row r="107" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A107" s="64"/>
       <c r="B107" s="62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>19</v>
@@ -10450,13 +10450,13 @@
       <c r="F107" s="4"/>
       <c r="G107" s="14"/>
     </row>
-    <row r="108" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A108" s="64"/>
       <c r="B108" s="62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>20</v>
@@ -10467,13 +10467,13 @@
       <c r="F108" s="4"/>
       <c r="G108" s="14"/>
     </row>
-    <row r="109" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="64"/>
       <c r="B109" s="62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>128</v>
@@ -10484,7 +10484,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="14"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="64"/>
       <c r="B110" s="39" t="s">
         <v>103</v>
@@ -10495,13 +10495,13 @@
       <c r="F110" s="47"/>
       <c r="G110" s="14"/>
     </row>
-    <row r="111" spans="1:7" ht="93.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="65"/>
       <c r="B111" s="63" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C111" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D111" s="49" t="s">
         <v>19</v>
@@ -10512,9 +10512,9 @@
       <c r="F111" s="49"/>
       <c r="G111" s="14"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B112" s="68" t="s">
         <v>125</v>
@@ -10525,13 +10525,13 @@
       <c r="F112" s="70"/>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A113" s="71"/>
       <c r="B113" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>20</v>
@@ -10541,13 +10541,13 @@
       </c>
       <c r="F113" s="4"/>
     </row>
-    <row r="114" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A114" s="71"/>
       <c r="B114" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>20</v>
@@ -10557,13 +10557,13 @@
       </c>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="72"/>
       <c r="B115" s="55" t="s">
+        <v>323</v>
+      </c>
+      <c r="C115" s="56" t="s">
         <v>324</v>
-      </c>
-      <c r="C115" s="56" t="s">
-        <v>325</v>
       </c>
       <c r="D115" s="56" t="s">
         <v>20</v>
@@ -10574,15 +10574,15 @@
       <c r="F115" s="56"/>
       <c r="G115" s="14"/>
     </row>
-    <row r="116" spans="1:7" ht="124" x14ac:dyDescent="0.35">
-      <c r="A116" s="83" t="s">
+    <row r="116" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A116" s="84" t="s">
         <v>23</v>
       </c>
       <c r="B116" s="43" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C116" s="44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D116" s="44" t="s">
         <v>19</v>
@@ -10593,13 +10593,13 @@
       <c r="F116" s="44"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="84"/>
+    <row r="117" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="85"/>
       <c r="B117" s="55" t="s">
+        <v>335</v>
+      </c>
+      <c r="C117" s="56" t="s">
         <v>336</v>
-      </c>
-      <c r="C117" s="56" t="s">
-        <v>337</v>
       </c>
       <c r="D117" s="56" t="s">
         <v>20</v>
@@ -10610,7 +10610,7 @@
       <c r="F117" s="56"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="64" t="s">
         <v>13</v>
       </c>
@@ -10623,10 +10623,10 @@
       <c r="F118" s="53"/>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="64"/>
       <c r="B119" s="62" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>82</v>
@@ -10640,10 +10640,10 @@
       <c r="F119" s="4"/>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="64"/>
       <c r="B120" s="62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>81</v>
@@ -10657,10 +10657,10 @@
       <c r="F120" s="4"/>
       <c r="G120" s="14"/>
     </row>
-    <row r="121" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="64"/>
       <c r="B121" s="62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>83</v>
@@ -10674,7 +10674,7 @@
       <c r="F121" s="4"/>
       <c r="G121" s="14"/>
     </row>
-    <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="64"/>
       <c r="B122" s="39" t="s">
         <v>105</v>
@@ -10685,13 +10685,13 @@
       <c r="F122" s="47"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="64"/>
       <c r="B123" s="62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>19</v>
@@ -10702,13 +10702,13 @@
       <c r="F123" s="4"/>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="64"/>
       <c r="B124" s="62" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>20</v>
@@ -10719,7 +10719,7 @@
       <c r="F124" s="4"/>
       <c r="G124" s="14"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="64"/>
       <c r="B125" s="39" t="s">
         <v>106</v>
@@ -10730,10 +10730,10 @@
       <c r="F125" s="47"/>
       <c r="G125" s="14"/>
     </row>
-    <row r="126" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="64"/>
       <c r="B126" s="62" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>67</v>
@@ -10747,13 +10747,13 @@
       <c r="F126" s="4"/>
       <c r="G126" s="14"/>
     </row>
-    <row r="127" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A127" s="64"/>
       <c r="B127" s="62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>19</v>
@@ -10764,7 +10764,7 @@
       <c r="F127" s="4"/>
       <c r="G127" s="14"/>
     </row>
-    <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="64"/>
       <c r="B128" s="39" t="s">
         <v>107</v>
@@ -10775,10 +10775,10 @@
       <c r="F128" s="47"/>
       <c r="G128" s="14"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="64"/>
       <c r="B129" s="62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>68</v>
@@ -10792,13 +10792,13 @@
       <c r="F129" s="4"/>
       <c r="G129" s="14"/>
     </row>
-    <row r="130" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="64"/>
       <c r="B130" s="62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D130" s="9" t="s">
         <v>20</v>
@@ -10809,7 +10809,7 @@
       <c r="F130" s="4"/>
       <c r="G130" s="14"/>
     </row>
-    <row r="131" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="64"/>
       <c r="B131" s="39" t="s">
         <v>108</v>
@@ -10820,13 +10820,13 @@
       <c r="F131" s="47"/>
       <c r="G131" s="14"/>
     </row>
-    <row r="132" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="126" x14ac:dyDescent="0.25">
       <c r="A132" s="64"/>
       <c r="B132" s="62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>20</v>
@@ -10837,7 +10837,7 @@
       <c r="F132" s="4"/>
       <c r="G132" s="14"/>
     </row>
-    <row r="133" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="64"/>
       <c r="B133" s="39" t="s">
         <v>109</v>
@@ -10848,10 +10848,10 @@
       <c r="F133" s="47"/>
       <c r="G133" s="14"/>
     </row>
-    <row r="134" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="64"/>
       <c r="B134" s="62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>25</v>
@@ -10865,10 +10865,10 @@
       <c r="F134" s="4"/>
       <c r="G134" s="14"/>
     </row>
-    <row r="135" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A135" s="64"/>
       <c r="B135" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>26</v>
@@ -10882,10 +10882,10 @@
       <c r="F135" s="4"/>
       <c r="G135" s="14"/>
     </row>
-    <row r="136" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A136" s="64"/>
       <c r="B136" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>69</v>
@@ -10899,10 +10899,10 @@
       <c r="F136" s="4"/>
       <c r="G136" s="14"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="64"/>
       <c r="B137" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>70</v>
@@ -10916,13 +10916,13 @@
       <c r="F137" s="4"/>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A138" s="64"/>
       <c r="B138" s="62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>128</v>
@@ -10933,10 +10933,10 @@
       <c r="F138" s="4"/>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A139" s="64"/>
       <c r="B139" s="62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>71</v>
@@ -10950,10 +10950,10 @@
       <c r="F139" s="4"/>
       <c r="G139" s="14"/>
     </row>
-    <row r="140" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A140" s="64"/>
       <c r="B140" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>27</v>
@@ -10967,13 +10967,13 @@
       <c r="F140" s="4"/>
       <c r="G140" s="14"/>
     </row>
-    <row r="141" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A141" s="64"/>
       <c r="B141" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>19</v>
@@ -10984,13 +10984,13 @@
       <c r="F141" s="4"/>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="65"/>
       <c r="B142" s="63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C142" s="54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D142" s="49" t="s">
         <v>20</v>
@@ -11001,12 +11001,12 @@
       <c r="F142" s="49"/>
       <c r="G142" s="14"/>
     </row>
-    <row r="143" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A143" s="81" t="s">
+    <row r="143" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A143" s="82" t="s">
         <v>24</v>
       </c>
       <c r="B143" s="43" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C143" s="44" t="s">
         <v>33</v>
@@ -11020,10 +11020,10 @@
       <c r="F143" s="44"/>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="81"/>
+    <row r="144" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A144" s="82"/>
       <c r="B144" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>34</v>
@@ -11037,10 +11037,10 @@
       <c r="F144" s="4"/>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A145" s="81"/>
+    <row r="145" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A145" s="82"/>
       <c r="B145" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>35</v>
@@ -11054,10 +11054,10 @@
       <c r="F145" s="4"/>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="81"/>
+    <row r="146" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A146" s="82"/>
       <c r="B146" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>36</v>
@@ -11071,10 +11071,10 @@
       <c r="F146" s="4"/>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A147" s="81"/>
+    <row r="147" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A147" s="82"/>
       <c r="B147" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>37</v>
@@ -11088,13 +11088,13 @@
       <c r="F147" s="4"/>
       <c r="G147" s="14"/>
     </row>
-    <row r="148" spans="1:7" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="82"/>
+    <row r="148" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="83"/>
       <c r="B148" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C148" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D148" s="49" t="s">
         <v>20</v>
@@ -11105,12 +11105,12 @@
       <c r="F148" s="49"/>
       <c r="G148" s="14"/>
     </row>
-    <row r="149" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A149" s="64" t="s">
         <v>14</v>
       </c>
       <c r="B149" s="66" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C149" s="44" t="s">
         <v>72</v>
@@ -11124,7 +11124,7 @@
       <c r="F149" s="44"/>
       <c r="G149" s="14"/>
     </row>
-    <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="64"/>
       <c r="B150" s="39" t="s">
         <v>110</v>
@@ -11135,10 +11135,10 @@
       <c r="F150" s="47"/>
       <c r="G150" s="14"/>
     </row>
-    <row r="151" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="64"/>
       <c r="B151" s="62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>73</v>
@@ -11152,10 +11152,10 @@
       <c r="F151" s="4"/>
       <c r="G151" s="14"/>
     </row>
-    <row r="152" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A152" s="64"/>
       <c r="B152" s="62" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>74</v>
@@ -11169,13 +11169,13 @@
       <c r="F152" s="4"/>
       <c r="G152" s="14"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="64"/>
       <c r="B153" s="62" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>20</v>
@@ -11186,13 +11186,13 @@
       <c r="F153" s="4"/>
       <c r="G153" s="14"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="64"/>
       <c r="B154" s="62" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>19</v>
@@ -11203,7 +11203,7 @@
       <c r="F154" s="4"/>
       <c r="G154" s="14"/>
     </row>
-    <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="64"/>
       <c r="B155" s="39" t="s">
         <v>111</v>
@@ -11214,10 +11214,10 @@
       <c r="F155" s="47"/>
       <c r="G155" s="14"/>
     </row>
-    <row r="156" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A156" s="64"/>
       <c r="B156" s="62" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>75</v>
@@ -11231,7 +11231,7 @@
       <c r="F156" s="4"/>
       <c r="G156" s="14"/>
     </row>
-    <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="64"/>
       <c r="B157" s="39" t="s">
         <v>112</v>
@@ -11242,10 +11242,10 @@
       <c r="F157" s="47"/>
       <c r="G157" s="14"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="64"/>
       <c r="B158" s="62" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>76</v>
@@ -11259,7 +11259,7 @@
       <c r="F158" s="4"/>
       <c r="G158" s="14"/>
     </row>
-    <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="64"/>
       <c r="B159" s="39" t="s">
         <v>113</v>
@@ -11270,10 +11270,10 @@
       <c r="F159" s="47"/>
       <c r="G159" s="14"/>
     </row>
-    <row r="160" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A160" s="64"/>
       <c r="B160" s="62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>38</v>
@@ -11287,10 +11287,10 @@
       <c r="F160" s="4"/>
       <c r="G160" s="14"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="64"/>
       <c r="B161" s="62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>39</v>
@@ -11304,10 +11304,10 @@
       <c r="F161" s="4"/>
       <c r="G161" s="14"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A162" s="64"/>
       <c r="B162" s="62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>84</v>
@@ -11321,7 +11321,7 @@
       <c r="F162" s="4"/>
       <c r="G162" s="14"/>
     </row>
-    <row r="163" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="64"/>
       <c r="B163" s="39" t="s">
         <v>114</v>
@@ -11332,10 +11332,10 @@
       <c r="F163" s="47"/>
       <c r="G163" s="14"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="64"/>
       <c r="B164" s="62" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>77</v>
@@ -11349,13 +11349,13 @@
       <c r="F164" s="4"/>
       <c r="G164" s="14"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="64"/>
       <c r="B165" s="62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>19</v>
@@ -11366,13 +11366,13 @@
       <c r="F165" s="4"/>
       <c r="G165" s="14"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A166" s="64"/>
       <c r="B166" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>19</v>
@@ -11383,10 +11383,10 @@
       <c r="F166" s="4"/>
       <c r="G166" s="14"/>
     </row>
-    <row r="167" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A167" s="64"/>
       <c r="B167" s="62" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>78</v>
@@ -11400,10 +11400,10 @@
       <c r="F167" s="4"/>
       <c r="G167" s="14"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="64"/>
       <c r="B168" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>40</v>
@@ -11417,13 +11417,13 @@
       <c r="F168" s="4"/>
       <c r="G168" s="14"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="64"/>
       <c r="B169" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>19</v>
@@ -11434,13 +11434,13 @@
       <c r="F169" s="4"/>
       <c r="G169" s="14"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="64"/>
       <c r="B170" s="74" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>19</v>
@@ -11451,7 +11451,7 @@
       <c r="F170" s="75"/>
       <c r="G170" s="14"/>
     </row>
-    <row r="171" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="64"/>
       <c r="B171" s="39" t="s">
         <v>115</v>
@@ -11462,13 +11462,13 @@
       <c r="F171" s="47"/>
       <c r="G171" s="14"/>
     </row>
-    <row r="172" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A172" s="64"/>
       <c r="B172" s="62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>19</v>
@@ -11479,10 +11479,10 @@
       <c r="F172" s="4"/>
       <c r="G172" s="14"/>
     </row>
-    <row r="173" spans="1:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="65"/>
       <c r="B173" s="63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C173" s="49" t="s">
         <v>41</v>
@@ -11496,7 +11496,7 @@
       <c r="F173" s="49"/>
       <c r="G173" s="14"/>
     </row>
-    <row r="174" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="64" t="s">
         <v>15</v>
       </c>
@@ -11509,13 +11509,13 @@
       <c r="F174" s="53"/>
       <c r="G174" s="14"/>
     </row>
-    <row r="175" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A175" s="64"/>
       <c r="B175" s="62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>19</v>
@@ -11526,10 +11526,10 @@
       <c r="F175" s="4"/>
       <c r="G175" s="14"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="64"/>
       <c r="B176" s="62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>42</v>
@@ -11543,10 +11543,10 @@
       <c r="F176" s="4"/>
       <c r="G176" s="14"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="64"/>
       <c r="B177" s="62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>28</v>
@@ -11560,13 +11560,13 @@
       <c r="F177" s="4"/>
       <c r="G177" s="14"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="64"/>
       <c r="B178" s="62" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>20</v>
@@ -11577,13 +11577,13 @@
       <c r="F178" s="4"/>
       <c r="G178" s="14"/>
     </row>
-    <row r="179" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A179" s="64"/>
       <c r="B179" s="62" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>20</v>
@@ -11594,7 +11594,7 @@
       <c r="F179" s="4"/>
       <c r="G179" s="14"/>
     </row>
-    <row r="180" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="64"/>
       <c r="B180" s="39" t="s">
         <v>16</v>
@@ -11605,13 +11605,13 @@
       <c r="F180" s="47"/>
       <c r="G180" s="14"/>
     </row>
-    <row r="181" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A181" s="64"/>
       <c r="B181" s="62" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>19</v>
@@ -11622,13 +11622,13 @@
       <c r="F181" s="4"/>
       <c r="G181" s="14"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="64"/>
       <c r="B182" s="62" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D182" s="4" t="s">
         <v>19</v>
@@ -11639,13 +11639,13 @@
       <c r="F182" s="4"/>
       <c r="G182" s="14"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="64"/>
       <c r="B183" s="62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>20</v>
@@ -11656,10 +11656,10 @@
       <c r="F183" s="4"/>
       <c r="G183" s="14"/>
     </row>
-    <row r="184" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="64"/>
       <c r="B184" s="62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>79</v>
@@ -11673,10 +11673,10 @@
       <c r="F184" s="4"/>
       <c r="G184" s="14"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="64"/>
       <c r="B185" s="62" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C185" s="5" t="s">
         <v>29</v>
@@ -11690,10 +11690,10 @@
       <c r="F185" s="4"/>
       <c r="G185" s="14"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A186" s="64"/>
       <c r="B186" s="62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>30</v>
@@ -11707,10 +11707,10 @@
       <c r="F186" s="4"/>
       <c r="G186" s="14"/>
     </row>
-    <row r="187" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A187" s="64"/>
       <c r="B187" s="62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>129</v>
@@ -11724,7 +11724,7 @@
       <c r="F187" s="4"/>
       <c r="G187" s="14"/>
     </row>
-    <row r="188" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="64"/>
       <c r="B188" s="39" t="s">
         <v>117</v>
@@ -11735,10 +11735,10 @@
       <c r="F188" s="47"/>
       <c r="G188" s="14"/>
     </row>
-    <row r="189" spans="1:7" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="65"/>
       <c r="B189" s="63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C189" s="49" t="s">
         <v>80</v>
@@ -11752,15 +11752,15 @@
       <c r="F189" s="49"/>
       <c r="G189" s="14"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B190" s="43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C190" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D190" s="44" t="s">
         <v>20</v>
@@ -11771,1369 +11771,1369 @@
       <c r="F190" s="46"/>
       <c r="G190" s="14"/>
     </row>
-    <row r="191" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="11"/>
       <c r="E191" s="33"/>
       <c r="F191" s="12"/>
       <c r="G191" s="12"/>
     </row>
-    <row r="192" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11"/>
       <c r="E192" s="33"/>
       <c r="F192" s="12"/>
       <c r="G192" s="12"/>
     </row>
-    <row r="193" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="11"/>
       <c r="E193" s="33"/>
       <c r="F193" s="12"/>
       <c r="G193" s="12"/>
     </row>
-    <row r="194" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="11"/>
       <c r="E194" s="33"/>
       <c r="F194" s="12"/>
       <c r="G194" s="12"/>
     </row>
-    <row r="195" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="11"/>
       <c r="E195" s="33"/>
       <c r="F195" s="12"/>
       <c r="G195" s="12"/>
     </row>
-    <row r="196" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="11"/>
       <c r="E196" s="33"/>
       <c r="F196" s="12"/>
       <c r="G196" s="12"/>
     </row>
-    <row r="197" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="11"/>
       <c r="E197" s="33"/>
       <c r="F197" s="12"/>
       <c r="G197" s="12"/>
     </row>
-    <row r="198" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="11"/>
       <c r="E198" s="33"/>
       <c r="F198" s="12"/>
       <c r="G198" s="12"/>
     </row>
-    <row r="199" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="11"/>
       <c r="E199" s="33"/>
       <c r="F199" s="12"/>
       <c r="G199" s="12"/>
     </row>
-    <row r="200" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="11"/>
       <c r="E200" s="33"/>
       <c r="F200" s="12"/>
       <c r="G200" s="12"/>
     </row>
-    <row r="201" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="11"/>
       <c r="E201" s="33"/>
       <c r="F201" s="12"/>
       <c r="G201" s="12"/>
     </row>
-    <row r="202" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="11"/>
       <c r="E202" s="33"/>
       <c r="F202" s="12"/>
       <c r="G202" s="12"/>
     </row>
-    <row r="203" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="11"/>
       <c r="E203" s="33"/>
       <c r="F203" s="12"/>
       <c r="G203" s="12"/>
     </row>
-    <row r="204" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="11"/>
       <c r="E204" s="33"/>
       <c r="F204" s="12"/>
       <c r="G204" s="12"/>
     </row>
-    <row r="205" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="11"/>
       <c r="E205" s="33"/>
       <c r="F205" s="12"/>
       <c r="G205" s="12"/>
     </row>
-    <row r="206" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="11"/>
       <c r="E206" s="33"/>
       <c r="F206" s="12"/>
       <c r="G206" s="12"/>
     </row>
-    <row r="207" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="11"/>
       <c r="E207" s="33"/>
       <c r="F207" s="12"/>
       <c r="G207" s="12"/>
     </row>
-    <row r="208" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="11"/>
       <c r="E208" s="33"/>
       <c r="F208" s="12"/>
       <c r="G208" s="12"/>
     </row>
-    <row r="209" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="11"/>
       <c r="E209" s="33"/>
       <c r="F209" s="12"/>
       <c r="G209" s="12"/>
     </row>
-    <row r="210" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="11"/>
       <c r="E210" s="33"/>
       <c r="F210" s="12"/>
       <c r="G210" s="12"/>
     </row>
-    <row r="211" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="11"/>
       <c r="E211" s="33"/>
       <c r="F211" s="12"/>
       <c r="G211" s="12"/>
     </row>
-    <row r="212" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="11"/>
       <c r="E212" s="33"/>
       <c r="F212" s="12"/>
       <c r="G212" s="12"/>
     </row>
-    <row r="213" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="11"/>
       <c r="E213" s="33"/>
       <c r="F213" s="12"/>
       <c r="G213" s="12"/>
     </row>
-    <row r="214" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="11"/>
       <c r="E214" s="33"/>
       <c r="F214" s="12"/>
       <c r="G214" s="12"/>
     </row>
-    <row r="215" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="11"/>
       <c r="E215" s="33"/>
       <c r="F215" s="12"/>
       <c r="G215" s="12"/>
     </row>
-    <row r="216" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="11"/>
       <c r="E216" s="33"/>
       <c r="F216" s="12"/>
       <c r="G216" s="12"/>
     </row>
-    <row r="217" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="11"/>
       <c r="E217" s="33"/>
       <c r="F217" s="12"/>
       <c r="G217" s="12"/>
     </row>
-    <row r="218" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="11"/>
       <c r="E218" s="33"/>
       <c r="F218" s="12"/>
       <c r="G218" s="12"/>
     </row>
-    <row r="219" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="11"/>
       <c r="E219" s="33"/>
       <c r="F219" s="12"/>
       <c r="G219" s="12"/>
     </row>
-    <row r="220" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="11"/>
       <c r="E220" s="33"/>
       <c r="F220" s="12"/>
       <c r="G220" s="12"/>
     </row>
-    <row r="221" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="11"/>
       <c r="E221" s="33"/>
       <c r="F221" s="12"/>
       <c r="G221" s="12"/>
     </row>
-    <row r="222" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="11"/>
       <c r="E222" s="33"/>
       <c r="F222" s="12"/>
       <c r="G222" s="12"/>
     </row>
-    <row r="223" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="11"/>
       <c r="E223" s="33"/>
       <c r="F223" s="12"/>
       <c r="G223" s="12"/>
     </row>
-    <row r="224" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="11"/>
       <c r="E224" s="33"/>
       <c r="F224" s="12"/>
       <c r="G224" s="12"/>
     </row>
-    <row r="225" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="11"/>
       <c r="E225" s="33"/>
       <c r="F225" s="12"/>
       <c r="G225" s="12"/>
     </row>
-    <row r="226" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="11"/>
       <c r="E226" s="33"/>
       <c r="F226" s="12"/>
       <c r="G226" s="12"/>
     </row>
-    <row r="227" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="11"/>
       <c r="E227" s="33"/>
       <c r="F227" s="12"/>
       <c r="G227" s="12"/>
     </row>
-    <row r="228" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="11"/>
       <c r="E228" s="33"/>
       <c r="F228" s="12"/>
       <c r="G228" s="12"/>
     </row>
-    <row r="229" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="11"/>
       <c r="E229" s="33"/>
       <c r="F229" s="12"/>
       <c r="G229" s="12"/>
     </row>
-    <row r="230" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="11"/>
       <c r="E230" s="33"/>
       <c r="F230" s="12"/>
       <c r="G230" s="12"/>
     </row>
-    <row r="231" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="11"/>
       <c r="E231" s="33"/>
       <c r="F231" s="12"/>
       <c r="G231" s="12"/>
     </row>
-    <row r="232" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="11"/>
       <c r="E232" s="33"/>
       <c r="F232" s="12"/>
       <c r="G232" s="12"/>
     </row>
-    <row r="233" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="11"/>
       <c r="E233" s="33"/>
       <c r="F233" s="12"/>
       <c r="G233" s="12"/>
     </row>
-    <row r="234" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="11"/>
       <c r="E234" s="33"/>
       <c r="F234" s="12"/>
       <c r="G234" s="12"/>
     </row>
-    <row r="235" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="11"/>
       <c r="E235" s="33"/>
       <c r="F235" s="12"/>
       <c r="G235" s="12"/>
     </row>
-    <row r="236" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="11"/>
       <c r="E236" s="33"/>
       <c r="F236" s="12"/>
       <c r="G236" s="12"/>
     </row>
-    <row r="237" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="11"/>
       <c r="E237" s="33"/>
       <c r="F237" s="12"/>
       <c r="G237" s="12"/>
     </row>
-    <row r="238" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="11"/>
       <c r="E238" s="33"/>
       <c r="F238" s="12"/>
       <c r="G238" s="12"/>
     </row>
-    <row r="239" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="11"/>
       <c r="E239" s="33"/>
       <c r="F239" s="12"/>
       <c r="G239" s="12"/>
     </row>
-    <row r="240" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="11"/>
       <c r="E240" s="33"/>
       <c r="F240" s="12"/>
       <c r="G240" s="12"/>
     </row>
-    <row r="241" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="11"/>
       <c r="E241" s="33"/>
       <c r="F241" s="12"/>
       <c r="G241" s="12"/>
     </row>
-    <row r="242" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="11"/>
       <c r="E242" s="33"/>
       <c r="F242" s="12"/>
       <c r="G242" s="12"/>
     </row>
-    <row r="243" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="11"/>
       <c r="E243" s="33"/>
       <c r="F243" s="12"/>
       <c r="G243" s="12"/>
     </row>
-    <row r="244" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="11"/>
       <c r="E244" s="33"/>
       <c r="F244" s="12"/>
       <c r="G244" s="12"/>
     </row>
-    <row r="245" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="11"/>
       <c r="E245" s="33"/>
       <c r="F245" s="12"/>
       <c r="G245" s="12"/>
     </row>
-    <row r="246" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="11"/>
       <c r="E246" s="33"/>
       <c r="F246" s="12"/>
       <c r="G246" s="12"/>
     </row>
-    <row r="247" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="11"/>
       <c r="E247" s="33"/>
       <c r="F247" s="12"/>
       <c r="G247" s="12"/>
     </row>
-    <row r="248" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="11"/>
       <c r="E248" s="33"/>
       <c r="F248" s="12"/>
       <c r="G248" s="12"/>
     </row>
-    <row r="249" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="11"/>
       <c r="E249" s="33"/>
       <c r="F249" s="12"/>
       <c r="G249" s="12"/>
     </row>
-    <row r="250" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="11"/>
       <c r="E250" s="33"/>
       <c r="F250" s="12"/>
       <c r="G250" s="12"/>
     </row>
-    <row r="251" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="11"/>
       <c r="E251" s="33"/>
       <c r="F251" s="12"/>
       <c r="G251" s="12"/>
     </row>
-    <row r="252" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="11"/>
       <c r="E252" s="33"/>
       <c r="F252" s="12"/>
       <c r="G252" s="12"/>
     </row>
-    <row r="253" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="11"/>
       <c r="E253" s="33"/>
       <c r="F253" s="12"/>
       <c r="G253" s="12"/>
     </row>
-    <row r="254" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="11"/>
       <c r="E254" s="33"/>
       <c r="F254" s="12"/>
       <c r="G254" s="12"/>
     </row>
-    <row r="255" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="11"/>
       <c r="E255" s="33"/>
       <c r="F255" s="12"/>
       <c r="G255" s="12"/>
     </row>
-    <row r="256" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="11"/>
       <c r="E256" s="33"/>
       <c r="F256" s="12"/>
       <c r="G256" s="12"/>
     </row>
-    <row r="257" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="11"/>
       <c r="E257" s="33"/>
       <c r="F257" s="12"/>
       <c r="G257" s="12"/>
     </row>
-    <row r="258" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="11"/>
       <c r="E258" s="33"/>
       <c r="F258" s="12"/>
       <c r="G258" s="12"/>
     </row>
-    <row r="259" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="11"/>
       <c r="E259" s="33"/>
       <c r="F259" s="12"/>
       <c r="G259" s="12"/>
     </row>
-    <row r="260" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="11"/>
       <c r="E260" s="33"/>
       <c r="F260" s="12"/>
       <c r="G260" s="12"/>
     </row>
-    <row r="261" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="11"/>
       <c r="E261" s="33"/>
       <c r="F261" s="12"/>
       <c r="G261" s="12"/>
     </row>
-    <row r="262" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="11"/>
       <c r="E262" s="33"/>
       <c r="F262" s="12"/>
       <c r="G262" s="12"/>
     </row>
-    <row r="263" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="11"/>
       <c r="E263" s="33"/>
       <c r="F263" s="12"/>
       <c r="G263" s="12"/>
     </row>
-    <row r="264" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="11"/>
       <c r="E264" s="33"/>
       <c r="F264" s="12"/>
       <c r="G264" s="12"/>
     </row>
-    <row r="265" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="11"/>
       <c r="E265" s="33"/>
       <c r="F265" s="12"/>
       <c r="G265" s="12"/>
     </row>
-    <row r="266" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="11"/>
       <c r="E266" s="33"/>
       <c r="F266" s="12"/>
       <c r="G266" s="12"/>
     </row>
-    <row r="267" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="11"/>
       <c r="E267" s="33"/>
       <c r="F267" s="12"/>
       <c r="G267" s="12"/>
     </row>
-    <row r="268" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="11"/>
       <c r="E268" s="33"/>
       <c r="F268" s="12"/>
       <c r="G268" s="12"/>
     </row>
-    <row r="269" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="11"/>
       <c r="E269" s="33"/>
       <c r="F269" s="12"/>
       <c r="G269" s="12"/>
     </row>
-    <row r="270" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="11"/>
       <c r="E270" s="33"/>
       <c r="F270" s="12"/>
       <c r="G270" s="12"/>
     </row>
-    <row r="271" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="11"/>
       <c r="E271" s="33"/>
       <c r="F271" s="12"/>
       <c r="G271" s="12"/>
     </row>
-    <row r="272" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" s="11"/>
       <c r="E272" s="33"/>
       <c r="F272" s="12"/>
       <c r="G272" s="12"/>
     </row>
-    <row r="273" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="11"/>
       <c r="E273" s="33"/>
       <c r="F273" s="12"/>
       <c r="G273" s="12"/>
     </row>
-    <row r="274" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="11"/>
       <c r="E274" s="33"/>
       <c r="F274" s="12"/>
       <c r="G274" s="12"/>
     </row>
-    <row r="275" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="11"/>
       <c r="E275" s="33"/>
       <c r="F275" s="12"/>
       <c r="G275" s="12"/>
     </row>
-    <row r="276" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="11"/>
       <c r="E276" s="33"/>
       <c r="F276" s="12"/>
       <c r="G276" s="12"/>
     </row>
-    <row r="277" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="11"/>
       <c r="E277" s="33"/>
       <c r="F277" s="12"/>
       <c r="G277" s="12"/>
     </row>
-    <row r="278" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="11"/>
       <c r="E278" s="33"/>
       <c r="F278" s="12"/>
       <c r="G278" s="12"/>
     </row>
-    <row r="279" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="11"/>
       <c r="E279" s="33"/>
       <c r="F279" s="12"/>
       <c r="G279" s="12"/>
     </row>
-    <row r="280" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" s="11"/>
       <c r="E280" s="33"/>
       <c r="F280" s="12"/>
       <c r="G280" s="12"/>
     </row>
-    <row r="281" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="11"/>
       <c r="E281" s="33"/>
       <c r="F281" s="12"/>
       <c r="G281" s="12"/>
     </row>
-    <row r="282" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="11"/>
       <c r="E282" s="33"/>
       <c r="F282" s="12"/>
       <c r="G282" s="12"/>
     </row>
-    <row r="283" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="11"/>
       <c r="E283" s="33"/>
       <c r="F283" s="12"/>
       <c r="G283" s="12"/>
     </row>
-    <row r="284" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="11"/>
       <c r="E284" s="33"/>
       <c r="F284" s="12"/>
       <c r="G284" s="12"/>
     </row>
-    <row r="285" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="11"/>
       <c r="E285" s="33"/>
       <c r="F285" s="12"/>
       <c r="G285" s="12"/>
     </row>
-    <row r="286" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="11"/>
       <c r="E286" s="33"/>
       <c r="F286" s="12"/>
       <c r="G286" s="12"/>
     </row>
-    <row r="287" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="11"/>
       <c r="E287" s="33"/>
       <c r="F287" s="12"/>
       <c r="G287" s="12"/>
     </row>
-    <row r="288" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="11"/>
       <c r="E288" s="33"/>
       <c r="F288" s="12"/>
       <c r="G288" s="12"/>
     </row>
-    <row r="289" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="11"/>
       <c r="E289" s="33"/>
       <c r="F289" s="12"/>
       <c r="G289" s="12"/>
     </row>
-    <row r="290" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="11"/>
       <c r="E290" s="33"/>
       <c r="F290" s="12"/>
       <c r="G290" s="12"/>
     </row>
-    <row r="291" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" s="11"/>
       <c r="E291" s="33"/>
       <c r="F291" s="12"/>
       <c r="G291" s="12"/>
     </row>
-    <row r="292" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="11"/>
       <c r="E292" s="33"/>
       <c r="F292" s="12"/>
       <c r="G292" s="12"/>
     </row>
-    <row r="293" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" s="11"/>
       <c r="E293" s="33"/>
       <c r="F293" s="12"/>
       <c r="G293" s="12"/>
     </row>
-    <row r="294" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" s="11"/>
       <c r="E294" s="33"/>
       <c r="F294" s="12"/>
       <c r="G294" s="12"/>
     </row>
-    <row r="295" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" s="11"/>
       <c r="E295" s="33"/>
       <c r="F295" s="12"/>
       <c r="G295" s="12"/>
     </row>
-    <row r="296" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A296" s="11"/>
       <c r="E296" s="33"/>
       <c r="F296" s="12"/>
       <c r="G296" s="12"/>
     </row>
-    <row r="297" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" s="11"/>
       <c r="E297" s="33"/>
       <c r="F297" s="12"/>
       <c r="G297" s="12"/>
     </row>
-    <row r="298" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A298" s="11"/>
       <c r="E298" s="33"/>
       <c r="F298" s="12"/>
       <c r="G298" s="12"/>
     </row>
-    <row r="299" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A299" s="11"/>
       <c r="E299" s="33"/>
       <c r="F299" s="12"/>
       <c r="G299" s="12"/>
     </row>
-    <row r="300" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A300" s="11"/>
       <c r="E300" s="33"/>
       <c r="F300" s="12"/>
       <c r="G300" s="12"/>
     </row>
-    <row r="301" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="11"/>
       <c r="E301" s="33"/>
       <c r="F301" s="12"/>
       <c r="G301" s="12"/>
     </row>
-    <row r="302" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A302" s="11"/>
       <c r="E302" s="33"/>
       <c r="F302" s="12"/>
       <c r="G302" s="12"/>
     </row>
-    <row r="303" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A303" s="11"/>
       <c r="E303" s="33"/>
       <c r="F303" s="12"/>
       <c r="G303" s="12"/>
     </row>
-    <row r="304" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" s="11"/>
       <c r="E304" s="33"/>
       <c r="F304" s="12"/>
       <c r="G304" s="12"/>
     </row>
-    <row r="305" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="11"/>
       <c r="E305" s="33"/>
       <c r="F305" s="12"/>
       <c r="G305" s="12"/>
     </row>
-    <row r="306" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" s="11"/>
       <c r="E306" s="33"/>
       <c r="F306" s="12"/>
       <c r="G306" s="12"/>
     </row>
-    <row r="307" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" s="11"/>
       <c r="E307" s="33"/>
       <c r="F307" s="12"/>
       <c r="G307" s="12"/>
     </row>
-    <row r="308" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" s="11"/>
       <c r="E308" s="33"/>
       <c r="F308" s="12"/>
       <c r="G308" s="12"/>
     </row>
-    <row r="309" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" s="11"/>
       <c r="E309" s="33"/>
       <c r="F309" s="12"/>
       <c r="G309" s="12"/>
     </row>
-    <row r="310" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" s="11"/>
       <c r="E310" s="33"/>
       <c r="F310" s="12"/>
       <c r="G310" s="12"/>
     </row>
-    <row r="311" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="11"/>
       <c r="E311" s="33"/>
       <c r="F311" s="12"/>
       <c r="G311" s="12"/>
     </row>
-    <row r="312" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A312" s="11"/>
       <c r="E312" s="33"/>
       <c r="F312" s="12"/>
       <c r="G312" s="12"/>
     </row>
-    <row r="313" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" s="11"/>
       <c r="E313" s="33"/>
       <c r="F313" s="12"/>
       <c r="G313" s="12"/>
     </row>
-    <row r="314" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="11"/>
       <c r="E314" s="33"/>
       <c r="F314" s="12"/>
       <c r="G314" s="12"/>
     </row>
-    <row r="315" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="11"/>
       <c r="E315" s="33"/>
       <c r="F315" s="12"/>
       <c r="G315" s="12"/>
     </row>
-    <row r="316" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" s="11"/>
       <c r="E316" s="33"/>
       <c r="F316" s="12"/>
       <c r="G316" s="12"/>
     </row>
-    <row r="317" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="11"/>
       <c r="E317" s="33"/>
       <c r="F317" s="12"/>
       <c r="G317" s="12"/>
     </row>
-    <row r="318" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="11"/>
       <c r="E318" s="33"/>
       <c r="F318" s="12"/>
       <c r="G318" s="12"/>
     </row>
-    <row r="319" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="11"/>
       <c r="E319" s="33"/>
       <c r="F319" s="12"/>
       <c r="G319" s="12"/>
     </row>
-    <row r="320" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="11"/>
       <c r="E320" s="33"/>
       <c r="F320" s="12"/>
       <c r="G320" s="12"/>
     </row>
-    <row r="321" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="11"/>
       <c r="E321" s="33"/>
       <c r="F321" s="12"/>
       <c r="G321" s="12"/>
     </row>
-    <row r="322" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="11"/>
       <c r="E322" s="33"/>
       <c r="F322" s="12"/>
       <c r="G322" s="12"/>
     </row>
-    <row r="323" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="11"/>
       <c r="E323" s="33"/>
       <c r="F323" s="12"/>
       <c r="G323" s="12"/>
     </row>
-    <row r="324" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A324" s="11"/>
       <c r="E324" s="33"/>
       <c r="F324" s="12"/>
       <c r="G324" s="12"/>
     </row>
-    <row r="325" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A325" s="11"/>
       <c r="E325" s="33"/>
       <c r="F325" s="12"/>
       <c r="G325" s="12"/>
     </row>
-    <row r="326" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A326" s="11"/>
       <c r="E326" s="33"/>
       <c r="F326" s="12"/>
       <c r="G326" s="12"/>
     </row>
-    <row r="327" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A327" s="11"/>
       <c r="E327" s="33"/>
       <c r="F327" s="12"/>
       <c r="G327" s="12"/>
     </row>
-    <row r="328" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A328" s="11"/>
       <c r="E328" s="33"/>
       <c r="F328" s="12"/>
       <c r="G328" s="12"/>
     </row>
-    <row r="329" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="11"/>
       <c r="E329" s="33"/>
       <c r="F329" s="12"/>
       <c r="G329" s="12"/>
     </row>
-    <row r="330" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="11"/>
       <c r="E330" s="33"/>
       <c r="F330" s="12"/>
       <c r="G330" s="12"/>
     </row>
-    <row r="331" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A331" s="11"/>
       <c r="E331" s="33"/>
       <c r="F331" s="12"/>
       <c r="G331" s="12"/>
     </row>
-    <row r="332" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="11"/>
       <c r="E332" s="33"/>
       <c r="F332" s="12"/>
       <c r="G332" s="12"/>
     </row>
-    <row r="333" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A333" s="11"/>
       <c r="E333" s="33"/>
       <c r="F333" s="12"/>
       <c r="G333" s="12"/>
     </row>
-    <row r="334" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="11"/>
       <c r="E334" s="33"/>
       <c r="F334" s="12"/>
       <c r="G334" s="12"/>
     </row>
-    <row r="335" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A335" s="11"/>
       <c r="E335" s="33"/>
       <c r="F335" s="12"/>
       <c r="G335" s="12"/>
     </row>
-    <row r="336" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A336" s="11"/>
       <c r="E336" s="33"/>
       <c r="F336" s="12"/>
       <c r="G336" s="12"/>
     </row>
-    <row r="337" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="11"/>
       <c r="E337" s="33"/>
       <c r="F337" s="12"/>
       <c r="G337" s="12"/>
     </row>
-    <row r="338" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A338" s="11"/>
       <c r="E338" s="33"/>
       <c r="F338" s="12"/>
       <c r="G338" s="12"/>
     </row>
-    <row r="339" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="11"/>
       <c r="E339" s="33"/>
       <c r="F339" s="12"/>
       <c r="G339" s="12"/>
     </row>
-    <row r="340" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="11"/>
       <c r="E340" s="33"/>
       <c r="F340" s="12"/>
       <c r="G340" s="12"/>
     </row>
-    <row r="341" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="11"/>
       <c r="E341" s="33"/>
       <c r="F341" s="12"/>
       <c r="G341" s="12"/>
     </row>
-    <row r="342" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A342" s="11"/>
       <c r="E342" s="33"/>
       <c r="F342" s="12"/>
       <c r="G342" s="12"/>
     </row>
-    <row r="343" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A343" s="11"/>
       <c r="E343" s="33"/>
       <c r="F343" s="12"/>
       <c r="G343" s="12"/>
     </row>
-    <row r="344" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A344" s="11"/>
       <c r="E344" s="33"/>
       <c r="F344" s="12"/>
       <c r="G344" s="12"/>
     </row>
-    <row r="345" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="11"/>
       <c r="E345" s="33"/>
       <c r="F345" s="12"/>
       <c r="G345" s="12"/>
     </row>
-    <row r="346" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="11"/>
       <c r="E346" s="33"/>
       <c r="F346" s="12"/>
       <c r="G346" s="12"/>
     </row>
-    <row r="347" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="11"/>
       <c r="E347" s="33"/>
       <c r="F347" s="12"/>
       <c r="G347" s="12"/>
     </row>
-    <row r="348" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="11"/>
       <c r="E348" s="33"/>
       <c r="F348" s="12"/>
       <c r="G348" s="12"/>
     </row>
-    <row r="349" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="11"/>
       <c r="E349" s="33"/>
       <c r="F349" s="12"/>
       <c r="G349" s="12"/>
     </row>
-    <row r="350" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="11"/>
       <c r="E350" s="33"/>
       <c r="F350" s="12"/>
       <c r="G350" s="12"/>
     </row>
-    <row r="351" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="11"/>
       <c r="E351" s="33"/>
       <c r="F351" s="12"/>
       <c r="G351" s="12"/>
     </row>
-    <row r="352" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="11"/>
       <c r="E352" s="33"/>
       <c r="F352" s="12"/>
       <c r="G352" s="12"/>
     </row>
-    <row r="353" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="11"/>
       <c r="E353" s="33"/>
       <c r="F353" s="12"/>
       <c r="G353" s="12"/>
     </row>
-    <row r="354" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="11"/>
       <c r="E354" s="33"/>
       <c r="F354" s="12"/>
       <c r="G354" s="12"/>
     </row>
-    <row r="355" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="11"/>
       <c r="E355" s="33"/>
       <c r="F355" s="12"/>
       <c r="G355" s="12"/>
     </row>
-    <row r="356" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="11"/>
       <c r="E356" s="33"/>
       <c r="F356" s="12"/>
       <c r="G356" s="12"/>
     </row>
-    <row r="357" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="11"/>
       <c r="E357" s="33"/>
       <c r="F357" s="12"/>
       <c r="G357" s="12"/>
     </row>
-    <row r="358" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="11"/>
       <c r="E358" s="33"/>
       <c r="F358" s="12"/>
       <c r="G358" s="12"/>
     </row>
-    <row r="359" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="11"/>
       <c r="E359" s="33"/>
       <c r="F359" s="12"/>
       <c r="G359" s="12"/>
     </row>
-    <row r="360" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="11"/>
       <c r="E360" s="33"/>
       <c r="F360" s="12"/>
       <c r="G360" s="12"/>
     </row>
-    <row r="361" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="11"/>
       <c r="E361" s="33"/>
       <c r="F361" s="12"/>
       <c r="G361" s="12"/>
     </row>
-    <row r="362" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="11"/>
       <c r="E362" s="33"/>
       <c r="F362" s="12"/>
       <c r="G362" s="12"/>
     </row>
-    <row r="363" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A363" s="11"/>
       <c r="E363" s="33"/>
       <c r="F363" s="12"/>
       <c r="G363" s="12"/>
     </row>
-    <row r="364" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A364" s="11"/>
       <c r="E364" s="33"/>
       <c r="F364" s="12"/>
       <c r="G364" s="12"/>
     </row>
-    <row r="365" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="11"/>
       <c r="E365" s="33"/>
       <c r="F365" s="12"/>
       <c r="G365" s="12"/>
     </row>
-    <row r="366" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A366" s="11"/>
       <c r="E366" s="33"/>
       <c r="F366" s="12"/>
       <c r="G366" s="12"/>
     </row>
-    <row r="367" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="11"/>
       <c r="E367" s="33"/>
       <c r="F367" s="12"/>
       <c r="G367" s="12"/>
     </row>
-    <row r="368" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="11"/>
       <c r="E368" s="33"/>
       <c r="F368" s="12"/>
       <c r="G368" s="12"/>
     </row>
-    <row r="369" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="11"/>
       <c r="E369" s="33"/>
       <c r="F369" s="12"/>
       <c r="G369" s="12"/>
     </row>
-    <row r="370" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="11"/>
       <c r="E370" s="33"/>
       <c r="F370" s="12"/>
       <c r="G370" s="12"/>
     </row>
-    <row r="371" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="11"/>
       <c r="E371" s="33"/>
       <c r="F371" s="12"/>
       <c r="G371" s="12"/>
     </row>
-    <row r="372" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="11"/>
       <c r="E372" s="33"/>
       <c r="F372" s="12"/>
       <c r="G372" s="12"/>
     </row>
-    <row r="373" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="11"/>
       <c r="E373" s="33"/>
       <c r="F373" s="12"/>
       <c r="G373" s="12"/>
     </row>
-    <row r="374" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="11"/>
       <c r="E374" s="33"/>
       <c r="F374" s="12"/>
       <c r="G374" s="12"/>
     </row>
-    <row r="375" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="11"/>
       <c r="E375" s="33"/>
       <c r="F375" s="12"/>
       <c r="G375" s="12"/>
     </row>
-    <row r="376" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="11"/>
       <c r="E376" s="33"/>
       <c r="F376" s="12"/>
       <c r="G376" s="12"/>
     </row>
-    <row r="377" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="11"/>
       <c r="E377" s="33"/>
       <c r="F377" s="12"/>
       <c r="G377" s="12"/>
     </row>
-    <row r="378" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="11"/>
       <c r="E378" s="33"/>
       <c r="F378" s="12"/>
       <c r="G378" s="12"/>
     </row>
-    <row r="379" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="11"/>
       <c r="E379" s="33"/>
       <c r="F379" s="12"/>
       <c r="G379" s="12"/>
     </row>
-    <row r="380" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="11"/>
       <c r="E380" s="33"/>
       <c r="F380" s="12"/>
       <c r="G380" s="12"/>
     </row>
-    <row r="381" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="11"/>
       <c r="E381" s="33"/>
       <c r="F381" s="12"/>
       <c r="G381" s="12"/>
     </row>
-    <row r="382" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A382" s="11"/>
       <c r="E382" s="33"/>
       <c r="F382" s="12"/>
       <c r="G382" s="12"/>
     </row>
-    <row r="383" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A383" s="11"/>
       <c r="E383" s="33"/>
       <c r="F383" s="12"/>
       <c r="G383" s="12"/>
     </row>
-    <row r="384" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A384" s="11"/>
       <c r="E384" s="33"/>
       <c r="F384" s="12"/>
       <c r="G384" s="12"/>
     </row>
-    <row r="385" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="11"/>
       <c r="E385" s="33"/>
       <c r="F385" s="12"/>
       <c r="G385" s="12"/>
     </row>
-    <row r="386" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="11"/>
       <c r="E386" s="33"/>
       <c r="F386" s="12"/>
       <c r="G386" s="12"/>
     </row>
-    <row r="387" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="11"/>
       <c r="E387" s="33"/>
       <c r="F387" s="12"/>
       <c r="G387" s="12"/>
     </row>
-    <row r="388" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="11"/>
       <c r="E388" s="33"/>
       <c r="F388" s="12"/>
       <c r="G388" s="12"/>
     </row>
-    <row r="389" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="11"/>
       <c r="E389" s="33"/>
       <c r="F389" s="12"/>
       <c r="G389" s="12"/>
     </row>
-    <row r="390" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="11"/>
       <c r="E390" s="33"/>
       <c r="F390" s="12"/>
       <c r="G390" s="12"/>
     </row>
-    <row r="391" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="11"/>
       <c r="E391" s="33"/>
       <c r="F391" s="12"/>
       <c r="G391" s="12"/>
     </row>
-    <row r="392" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="11"/>
       <c r="E392" s="33"/>
       <c r="F392" s="12"/>
       <c r="G392" s="12"/>
     </row>
-    <row r="393" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="11"/>
       <c r="E393" s="33"/>
       <c r="F393" s="12"/>
       <c r="G393" s="12"/>
     </row>
-    <row r="394" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="11"/>
       <c r="E394" s="33"/>
       <c r="F394" s="12"/>
       <c r="G394" s="12"/>
     </row>
-    <row r="395" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="11"/>
       <c r="E395" s="33"/>
       <c r="F395" s="12"/>
       <c r="G395" s="12"/>
     </row>
-    <row r="396" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="11"/>
       <c r="E396" s="33"/>
       <c r="F396" s="12"/>
       <c r="G396" s="12"/>
     </row>
-    <row r="397" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="11"/>
       <c r="E397" s="33"/>
       <c r="F397" s="12"/>
       <c r="G397" s="12"/>
     </row>
-    <row r="398" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="11"/>
       <c r="E398" s="33"/>
       <c r="F398" s="12"/>
       <c r="G398" s="12"/>
     </row>
-    <row r="399" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="11"/>
       <c r="E399" s="33"/>
       <c r="F399" s="12"/>
       <c r="G399" s="12"/>
     </row>
-    <row r="400" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A400" s="11"/>
       <c r="E400" s="33"/>
       <c r="F400" s="12"/>
       <c r="G400" s="12"/>
     </row>
-    <row r="401" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A401" s="11"/>
       <c r="E401" s="33"/>
       <c r="F401" s="12"/>
       <c r="G401" s="12"/>
     </row>
-    <row r="402" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A402" s="11"/>
       <c r="E402" s="33"/>
       <c r="F402" s="12"/>
       <c r="G402" s="12"/>
     </row>
-    <row r="403" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A403" s="11"/>
       <c r="E403" s="33"/>
       <c r="F403" s="12"/>
       <c r="G403" s="12"/>
     </row>
-    <row r="404" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A404" s="11"/>
       <c r="E404" s="33"/>
       <c r="F404" s="12"/>
       <c r="G404" s="12"/>
     </row>
-    <row r="405" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A405" s="11"/>
       <c r="E405" s="33"/>
       <c r="F405" s="12"/>
       <c r="G405" s="12"/>
     </row>
-    <row r="406" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A406" s="11"/>
       <c r="E406" s="33"/>
       <c r="F406" s="12"/>
       <c r="G406" s="12"/>
     </row>
-    <row r="407" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A407" s="11"/>
       <c r="E407" s="33"/>
       <c r="F407" s="12"/>
       <c r="G407" s="12"/>
     </row>
-    <row r="408" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A408" s="11"/>
       <c r="E408" s="33"/>
       <c r="F408" s="12"/>
       <c r="G408" s="12"/>
     </row>
-    <row r="409" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A409" s="11"/>
       <c r="E409" s="33"/>
       <c r="F409" s="12"/>
       <c r="G409" s="12"/>
     </row>
-    <row r="410" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A410" s="11"/>
       <c r="E410" s="33"/>
       <c r="F410" s="12"/>
       <c r="G410" s="12"/>
     </row>
-    <row r="411" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A411" s="11"/>
       <c r="E411" s="33"/>
       <c r="F411" s="12"/>
       <c r="G411" s="12"/>
     </row>
-    <row r="412" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A412" s="11"/>
       <c r="E412" s="33"/>
       <c r="F412" s="12"/>
       <c r="G412" s="12"/>
     </row>
-    <row r="413" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A413" s="11"/>
       <c r="E413" s="33"/>
       <c r="F413" s="12"/>
       <c r="G413" s="12"/>
     </row>
-    <row r="414" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A414" s="11"/>
       <c r="E414" s="33"/>
       <c r="F414" s="12"/>
       <c r="G414" s="12"/>
     </row>
-    <row r="415" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A415" s="11"/>
       <c r="E415" s="33"/>
       <c r="F415" s="12"/>
       <c r="G415" s="12"/>
     </row>
-    <row r="416" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A416" s="11"/>
       <c r="E416" s="33"/>
       <c r="F416" s="12"/>
       <c r="G416" s="12"/>
     </row>
-    <row r="417" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A417" s="11"/>
       <c r="E417" s="33"/>
       <c r="F417" s="12"/>
       <c r="G417" s="12"/>
     </row>
-    <row r="418" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A418" s="11"/>
       <c r="E418" s="33"/>
       <c r="F418" s="12"/>
@@ -13222,26 +13222,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <g8cc7f6e98b34d1387cc1791a9d2d9a3 xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g8cc7f6e98b34d1387cc1791a9d2d9a3>
-    <MSB_RecordId xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f" xsi:nil="true"/>
-    <l327da1f1d44497ab3337057f4d04951 xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Standard</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">42db7290-f92b-446b-999c-1bee6d848af0</TermId>
-        </TermInfo>
-      </Terms>
-    </l327da1f1d44497ab3337057f4d04951>
-    <msbLabel xmlns="09080109-f6cd-4eba-a2ee-73217fe696ed"/>
-    <TaxCatchAll xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
-      <Value>1</Value>
-    </TaxCatchAll>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13456,27 +13442,32 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <g8cc7f6e98b34d1387cc1791a9d2d9a3 xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g8cc7f6e98b34d1387cc1791a9d2d9a3>
+    <MSB_RecordId xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f" xsi:nil="true"/>
+    <l327da1f1d44497ab3337057f4d04951 xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Standard</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">42db7290-f92b-446b-999c-1bee6d848af0</TermId>
+        </TermInfo>
+      </Terms>
+    </l327da1f1d44497ab3337057f4d04951>
+    <msbLabel xmlns="09080109-f6cd-4eba-a2ee-73217fe696ed"/>
+    <TaxCatchAll xmlns="06622f86-497a-49b5-9d4e-f3ea00047d2f">
+      <Value>1</Value>
+    </TaxCatchAll>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6189EC1A-B24C-4E26-AA9F-67A591DDE31F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74E39A40-EF53-41B0-AE0C-BDF1760CF50B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="06622f86-497a-49b5-9d4e-f3ea00047d2f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="09080109-f6cd-4eba-a2ee-73217fe696ed"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13501,9 +13492,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74E39A40-EF53-41B0-AE0C-BDF1760CF50B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6189EC1A-B24C-4E26-AA9F-67A591DDE31F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="06622f86-497a-49b5-9d4e-f3ea00047d2f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="09080109-f6cd-4eba-a2ee-73217fe696ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>